<commit_message>
Added back in 2010-2012 because why not
also made it so the notebook can run through all the cells without errors
</commit_message>
<xml_diff>
--- a/yearly_death_totals.xlsx
+++ b/yearly_death_totals.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Douglas\Documents\Spring_23\cs484\project\FentanylFighters-doug\useful_features\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Douglas\Documents\GitHub\FentanylFighters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A1B627F-DE18-4221-A594-4BB5D2D34398}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BDA4A6E-CCBD-4385-90B6-6C6C950C468D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="15196" xr2:uid="{D125F9EB-F5A0-4639-A64D-32970EB16C29}"/>
+    <workbookView xWindow="11250" yWindow="0" windowWidth="11250" windowHeight="15000" xr2:uid="{D125F9EB-F5A0-4639-A64D-32970EB16C29}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -382,63 +382,81 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BBB7C99-DD78-48D3-BFFF-39009E875A2D}">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A1">
+        <v>2010</v>
+      </c>
+      <c r="B1">
+        <v>2011</v>
+      </c>
+      <c r="C1">
+        <v>2012</v>
+      </c>
+      <c r="D1">
         <v>2013</v>
       </c>
-      <c r="B1">
+      <c r="E1">
         <v>2014</v>
       </c>
-      <c r="C1">
+      <c r="F1">
         <v>2015</v>
       </c>
-      <c r="D1">
+      <c r="G1">
         <v>2016</v>
       </c>
-      <c r="E1">
+      <c r="H1">
         <v>2017</v>
       </c>
-      <c r="F1">
+      <c r="I1">
         <v>2018</v>
       </c>
-      <c r="G1">
+      <c r="J1">
         <v>2019</v>
       </c>
-      <c r="H1">
+      <c r="K1">
         <v>2020</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A2">
+        <v>19983</v>
+      </c>
+      <c r="B2">
+        <v>21414</v>
+      </c>
+      <c r="C2">
+        <v>21837</v>
+      </c>
+      <c r="D2">
         <v>24005</v>
       </c>
-      <c r="B2">
+      <c r="E2">
         <v>28015</v>
       </c>
-      <c r="C2">
+      <c r="F2">
         <v>32493</v>
       </c>
-      <c r="D2">
+      <c r="G2">
         <v>41918</v>
       </c>
-      <c r="E2">
+      <c r="H2">
         <v>47576</v>
       </c>
-      <c r="F2">
+      <c r="I2">
         <v>47118</v>
       </c>
-      <c r="G2">
+      <c r="J2">
         <v>50384</v>
       </c>
-      <c r="H2">
+      <c r="K2">
         <v>69432</v>
       </c>
     </row>

</xml_diff>